<commit_message>
issue70: Create GrAE staking lifecycle diagram
</commit_message>
<xml_diff>
--- a/general-content/solanaSSliquidityNeeds.xlsx
+++ b/general-content/solanaSSliquidityNeeds.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blairmunroakusa/_ROOT/interlockDUMP/ILOCK-smartcontracts/general-content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C45549-EA72-1D4C-B3AF-72E9377E3D00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC29D19-1190-0944-854C-DA345AF8CFD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="500" windowWidth="37740" windowHeight="23500" xr2:uid="{60E725C3-AD31-1746-8586-B258B1159DDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -100,8 +100,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="0.00000000"/>
-    <numFmt numFmtId="175" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -385,22 +385,19 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -408,12 +405,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -434,7 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -443,26 +434,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -478,6 +454,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -794,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15333263-B99C-0C4D-BA8A-79D53CD1DB7B}">
-  <dimension ref="B2:Y22"/>
+  <dimension ref="B2:Y33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,415 +822,415 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:21" s="8" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9"/>
+    <row r="3" spans="2:21" s="7" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8"/>
     </row>
     <row r="4" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="21"/>
-      <c r="K4" s="12"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="18"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B5" s="18"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="15" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="21"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="18"/>
     </row>
     <row r="6" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="37">
+      <c r="B6" s="16"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="49">
         <v>10000</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="40">
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="47">
         <v>100000</v>
       </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="40">
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="47">
         <v>1000000</v>
       </c>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="21"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="18"/>
     </row>
     <row r="7" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="35" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="34">
+      <c r="D7" s="46"/>
+      <c r="E7" s="31">
         <v>1000</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="31">
         <v>10000</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="31">
         <v>100000</v>
       </c>
-      <c r="H7" s="45"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="34">
+      <c r="H7" s="37"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="31">
         <v>1000</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7" s="31">
         <v>10000</v>
       </c>
-      <c r="L7" s="34">
+      <c r="L7" s="31">
         <v>100000</v>
       </c>
-      <c r="M7" s="34">
+      <c r="M7" s="31">
         <v>1000000</v>
       </c>
-      <c r="N7" s="34"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="34">
+      <c r="N7" s="31"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="31">
         <v>10000</v>
       </c>
-      <c r="Q7" s="34">
+      <c r="Q7" s="31">
         <v>100000</v>
       </c>
-      <c r="R7" s="34">
+      <c r="R7" s="31">
         <v>1000000</v>
       </c>
-      <c r="S7" s="34">
+      <c r="S7" s="31">
         <v>10000000</v>
       </c>
-      <c r="T7" s="33"/>
-      <c r="U7" s="21"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="18"/>
     </row>
     <row r="8" spans="2:21" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="21"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="18"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="32">
         <v>1000</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="42">
+      <c r="D9" s="18"/>
+      <c r="E9" s="34">
         <f>(E7*Y21)+(E6*Y20)+(C9*Y22)</f>
         <v>1893.12</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="34">
         <f>E6*Y20+F7*Y21+C9*Y22</f>
         <v>3120.864</v>
       </c>
-      <c r="G9" s="42">
+      <c r="G9" s="34">
         <f>E6*Y20+G7*Y21+C9*Y22</f>
         <v>15398.303999999998</v>
       </c>
-      <c r="H9" s="47"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42">
+      <c r="H9" s="39"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34">
         <f>J6*Y20+J7*Y21+C9*Y22</f>
         <v>16425.599999999999</v>
       </c>
-      <c r="K9" s="42">
+      <c r="K9" s="34">
         <f>J6*Y20+K7*Y21+C9*Y22</f>
         <v>17653.344000000001</v>
       </c>
-      <c r="L9" s="42">
+      <c r="L9" s="34">
         <f>J6*Y20+L7*Y21+C9*Y22</f>
         <v>29930.784</v>
       </c>
-      <c r="M9" s="42">
+      <c r="M9" s="34">
         <f>J6*Y20+M7*Y21+C9*Y22</f>
         <v>152705.18399999998</v>
       </c>
-      <c r="N9" s="42"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="42">
+      <c r="N9" s="34"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="34">
         <f>P6*Y20+P7*Y21+C9*Y22</f>
         <v>162978.144</v>
       </c>
-      <c r="Q9" s="42">
+      <c r="Q9" s="34">
         <f>P6*Y20+Q7*Y21+C9*Y22</f>
         <v>175255.584</v>
       </c>
-      <c r="R9" s="42">
+      <c r="R9" s="34">
         <f>P6*Y20+R7*Y21+C9*Y22</f>
         <v>298029.984</v>
       </c>
-      <c r="S9" s="42">
+      <c r="S9" s="34">
         <f>P6*Y20+S7*Y21+C9*Y22</f>
         <v>1525773.9839999997</v>
       </c>
-      <c r="T9" s="13"/>
-      <c r="U9" s="21"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="18"/>
     </row>
     <row r="10" spans="2:21" ht="7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="41"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="42"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="21"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="18"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B11" s="41"/>
-      <c r="C11" s="38">
+      <c r="B11" s="48"/>
+      <c r="C11" s="32">
         <v>10000</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="42">
+      <c r="D11" s="18"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="34">
         <f>E6*Y20+F7*Y21+C11*Y22</f>
         <v>4398.72</v>
       </c>
-      <c r="G11" s="42">
+      <c r="G11" s="34">
         <f>E6*Y20+G7*Y21+C11*Y22</f>
         <v>16676.159999999996</v>
       </c>
-      <c r="H11" s="47"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="42">
+      <c r="H11" s="39"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="34">
         <f>J6*Y20+K7*Y21+C11*Y22</f>
         <v>18931.2</v>
       </c>
-      <c r="L11" s="42">
+      <c r="L11" s="34">
         <f>J6*Y20+L7*Y21+C11*Y22</f>
         <v>31208.639999999999</v>
       </c>
-      <c r="M11" s="42">
+      <c r="M11" s="34">
         <f>J6*Y20+M7*Y21+C11*Y22</f>
         <v>153983.03999999998</v>
       </c>
-      <c r="N11" s="42"/>
-      <c r="O11" s="51"/>
-      <c r="P11" s="42">
+      <c r="N11" s="34"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="34">
         <f>P6*Y20+P7*Y21+C11*Y22</f>
         <v>164256</v>
       </c>
-      <c r="Q11" s="42">
+      <c r="Q11" s="34">
         <f>P6*Y20+Q7*Y21+C11*Y22</f>
         <v>176533.44</v>
       </c>
-      <c r="R11" s="42">
+      <c r="R11" s="34">
         <f>P6*Y20+R7*Y21+C11*Y22</f>
         <v>299307.84000000003</v>
       </c>
-      <c r="S11" s="42">
+      <c r="S11" s="34">
         <f>P6*Y20+S7*Y21+C11*Y22</f>
         <v>1527051.8399999999</v>
       </c>
-      <c r="T11" s="13"/>
-      <c r="U11" s="21"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="18"/>
     </row>
     <row r="12" spans="2:21" ht="7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="41"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="21"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="18"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B13" s="41"/>
-      <c r="C13" s="38">
+      <c r="B13" s="48"/>
+      <c r="C13" s="32">
         <v>100000</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="42">
+      <c r="D13" s="18"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="34">
         <f>E6*Y20+G7*Y21+C13*Y22</f>
         <v>29454.719999999998</v>
       </c>
-      <c r="H13" s="47"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="42">
+      <c r="H13" s="39"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="34">
         <f>J6*Y20+L7*Y21+C13*Y22</f>
         <v>43987.199999999997</v>
       </c>
-      <c r="M13" s="42">
+      <c r="M13" s="34">
         <f>J6*Y20+M7*Y21+C13*Y22</f>
         <v>166761.59999999998</v>
       </c>
-      <c r="N13" s="42"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="42">
+      <c r="N13" s="34"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="34">
         <f>P6*Y20+Q7*Y21+C13*Y22</f>
         <v>189312</v>
       </c>
-      <c r="R13" s="42">
+      <c r="R13" s="34">
         <f>P6*Y20+R7*Y21+C13*Y22</f>
         <v>312086.40000000002</v>
       </c>
-      <c r="S13" s="42">
+      <c r="S13" s="34">
         <f>P6*Y20+S7*Y21+C13*Y22</f>
         <v>1539830.3999999997</v>
       </c>
-      <c r="T13" s="13"/>
-      <c r="U13" s="21"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="18"/>
     </row>
     <row r="14" spans="2:21" ht="7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="41"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="43"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="21"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="18"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B15" s="41"/>
-      <c r="C15" s="38">
+      <c r="B15" s="48"/>
+      <c r="C15" s="32">
         <v>1000000</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="42">
+      <c r="D15" s="18"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="34">
         <f>J6*Y20+M7*Y21+C15*Y22</f>
         <v>294547.19999999995</v>
       </c>
-      <c r="N15" s="42"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="43"/>
-      <c r="R15" s="42">
+      <c r="N15" s="34"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="34">
         <f>P6*Y20+R7*Y21+C15*Y22</f>
         <v>439872</v>
       </c>
-      <c r="S15" s="42">
+      <c r="S15" s="34">
         <f>P6*Y20+S7*Y21+C15*Y22</f>
         <v>1667615.9999999998</v>
       </c>
-      <c r="T15" s="13"/>
-      <c r="U15" s="21"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="18"/>
     </row>
     <row r="16" spans="2:21" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="21"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="18"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B17" s="11"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="9"/>
       <c r="U17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V17" s="5">
+      <c r="V17" s="4">
         <v>100</v>
       </c>
       <c r="W17" t="s">
@@ -1240,10 +1241,10 @@
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="X18" s="3" t="s">
+      <c r="X18" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="Y18" s="3"/>
+      <c r="Y18" s="51"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
@@ -1252,14 +1253,14 @@
       <c r="U19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V19" s="3" t="s">
+      <c r="V19" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="W19" s="3"/>
-      <c r="X19" s="4" t="s">
+      <c r="W19" s="51"/>
+      <c r="X19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Y19" s="6" t="s">
+      <c r="Y19" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1279,7 +1280,7 @@
       <c r="X20">
         <v>1.61472E-3</v>
       </c>
-      <c r="Y20" s="7">
+      <c r="Y20" s="6">
         <f>X20*V17</f>
         <v>0.161472</v>
       </c>
@@ -1300,7 +1301,7 @@
       <c r="X21">
         <v>1.3641599999999999E-3</v>
       </c>
-      <c r="Y21" s="7">
+      <c r="Y21" s="6">
         <f>X21*V17</f>
         <v>0.13641599999999998</v>
       </c>
@@ -1321,21 +1322,24 @@
       <c r="X22">
         <v>1.4198399999999999E-3</v>
       </c>
-      <c r="Y22" s="7">
+      <c r="Y22" s="6">
         <f>X22*V17</f>
         <v>0.141984</v>
       </c>
     </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="52"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="X18:Y18"/>
     <mergeCell ref="E5:S5"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="E6:G6"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="X18:Y18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>